<commit_message>
adding new data to excel and set sheet in script
</commit_message>
<xml_diff>
--- a/arquivos/excelEmrpesa.xlsx
+++ b/arquivos/excelEmrpesa.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caroline\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caroline\Analise-de-Dados\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D4DF07-8F92-4D7F-BE93-C5DFACFC5AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F31F0B-8D47-4CFC-AA76-DE3DF95499E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E71AEBCC-7E7E-41BC-969A-A8008FE28960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E71AEBCC-7E7E-41BC-969A-A8008FE28960}"/>
   </bookViews>
   <sheets>
-    <sheet name="Novembro - 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Outubro - 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Novembro - 2024" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Novembro - 2024'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Novembro - 2024'!$A$1:$E$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Outubro - 2024'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="171">
   <si>
     <t>Nome da Cliente</t>
   </si>
@@ -243,44 +245,399 @@
     <t>Total no mês</t>
   </si>
   <si>
-    <t xml:space="preserve"> 8/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16/11/24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17/11/24 </t>
+    <t>Carolina Almeida</t>
+  </si>
+  <si>
+    <t>Juliana Martins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatiane Souza </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cílios Egípcio  </t>
+  </si>
+  <si>
+    <t>Lash Lifting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simone Costa      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raquel Oliveira     </t>
+  </si>
+  <si>
+    <t>Gabriela Almeida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanessa Ferreira </t>
+  </si>
+  <si>
+    <t>Mariana Costa</t>
+  </si>
+  <si>
+    <t>Clara Lima</t>
+  </si>
+  <si>
+    <t>Patrícia Silva</t>
+  </si>
+  <si>
+    <t>Alice Costa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aline Souza  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renata Costa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriela Rocha    </t>
+  </si>
+  <si>
+    <t>20/11/24</t>
+  </si>
+  <si>
+    <t>Letícia Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberta Pereira   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joana Oliveira  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larissa Santos     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bianca Lima        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabiana Almeida   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paula Costa         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruna Lima          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marta Oliveira  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carol Martins </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jéssica Almeida  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabrina Silva     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabiane Costa  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elisa Martins        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viviane Ferreira     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larissa Costa      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanessa Rocha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabel Santos      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simone Martins   </t>
+  </si>
+  <si>
+    <t>Karina Almeida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatiane Santos </t>
+  </si>
+  <si>
+    <t>Camila Costa</t>
+  </si>
+  <si>
+    <t>Thais Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andressa Pereira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sara Lima  </t>
+  </si>
+  <si>
+    <t>Daniela Souza</t>
+  </si>
+  <si>
+    <t>13/10/24</t>
+  </si>
+  <si>
+    <t>14/10/24</t>
+  </si>
+  <si>
+    <t>15/10/24</t>
+  </si>
+  <si>
+    <t>16/10/24</t>
+  </si>
+  <si>
+    <t>17/10/24</t>
+  </si>
+  <si>
+    <t>18/10/24</t>
+  </si>
+  <si>
+    <t>19/10/24</t>
+  </si>
+  <si>
+    <t>20/10/24</t>
+  </si>
+  <si>
+    <t>21/10/24</t>
+  </si>
+  <si>
+    <t>22/10/24</t>
+  </si>
+  <si>
+    <t>23/10/24</t>
+  </si>
+  <si>
+    <t>24/10/24</t>
+  </si>
+  <si>
+    <t>25/10/24</t>
+  </si>
+  <si>
+    <t>26/10/2024</t>
+  </si>
+  <si>
+    <t>27/10/2024</t>
+  </si>
+  <si>
+    <t>28/10/2024</t>
+  </si>
+  <si>
+    <t>29/10/2024</t>
+  </si>
+  <si>
+    <t>30/10/2024</t>
+  </si>
+  <si>
+    <t>Fátima Almeida</t>
+  </si>
+  <si>
+    <t>Marcela Santos</t>
+  </si>
+  <si>
+    <t>Paula Nunes</t>
+  </si>
+  <si>
+    <t>Angela Costa</t>
+  </si>
+  <si>
+    <t>Débora Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita Barbosa   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adriana Silva   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edna Pereira   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raquel Lima      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letícia Almeida  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bianca Rocha    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simone Farias        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viviane Lima  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafaela Costa        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manuela Souza      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giselle Pereira     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Natália Farias       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camila Silva       </t>
+  </si>
+  <si>
+    <t>13/11/24</t>
+  </si>
+  <si>
+    <t>14/11/24</t>
+  </si>
+  <si>
+    <t>Juliana Oliveira</t>
+  </si>
+  <si>
+    <t>Fernanda Ribeiro</t>
+  </si>
+  <si>
+    <t>Larissa Martins</t>
+  </si>
+  <si>
+    <t>Isabela Andrade</t>
+  </si>
+  <si>
+    <t>Marcela Costa</t>
+  </si>
+  <si>
+    <t>Renata Alves</t>
+  </si>
+  <si>
+    <t>Rafaela Melo</t>
+  </si>
+  <si>
+    <r>
+      <t>Ana Lima</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Patrícia Menezes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Carla Duarte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tatiana Rocha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aline Cardoso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cristina Silva</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Beatriz Teixeira</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>15/11/24</t>
+  </si>
+  <si>
+    <t>16/11/24</t>
+  </si>
+  <si>
+    <t>17/11/24</t>
+  </si>
+  <si>
+    <t>18/11/24</t>
+  </si>
+  <si>
+    <t>19/11/24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="166" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -360,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -386,16 +743,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -407,14 +758,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -731,20 +1102,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B403C4-EB86-4989-8F89-81F8E5514A26}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -756,16 +1127,16 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -776,18 +1147,18 @@
       <c r="B2" s="3">
         <v>28</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="17">
         <v>150</v>
       </c>
-      <c r="E2" s="16">
-        <v>45302</v>
-      </c>
-      <c r="F2" s="12">
-        <f>SUM(B3:B52)</f>
-        <v>1405</v>
+      <c r="E2" s="14">
+        <v>45301</v>
+      </c>
+      <c r="F2" s="18">
+        <f>SUM(D2:D94)</f>
+        <v>16660</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -797,14 +1168,14 @@
       <c r="B3" s="3">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="17">
         <v>200</v>
       </c>
-      <c r="E3" s="16">
-        <v>45302</v>
+      <c r="E3" s="14">
+        <v>45301</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -814,14 +1185,14 @@
       <c r="B4" s="3">
         <v>34</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="17">
         <v>100</v>
       </c>
-      <c r="E4" s="16">
-        <v>45302</v>
+      <c r="E4" s="14">
+        <v>45301</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,14 +1202,14 @@
       <c r="B5" s="3">
         <v>30</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="17">
         <v>180</v>
       </c>
-      <c r="E5" s="16">
-        <v>45333</v>
+      <c r="E5" s="14">
+        <v>45332</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,14 +1219,14 @@
       <c r="B6" s="3">
         <v>21</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="17">
         <v>220</v>
       </c>
-      <c r="E6" s="16">
-        <v>45333</v>
+      <c r="E6" s="14">
+        <v>45332</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,14 +1236,14 @@
       <c r="B7" s="3">
         <v>40</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="17">
         <v>200</v>
       </c>
-      <c r="E7" s="16">
-        <v>45333</v>
+      <c r="E7" s="14">
+        <v>45332</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,14 +1253,14 @@
       <c r="B8" s="3">
         <v>25</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="17">
         <v>190</v>
       </c>
-      <c r="E8" s="16">
-        <v>45362</v>
+      <c r="E8" s="14">
+        <v>45361</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,14 +1270,14 @@
       <c r="B9" s="3">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="17">
         <v>180</v>
       </c>
-      <c r="E9" s="16">
-        <v>45362</v>
+      <c r="E9" s="14">
+        <v>45361</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,14 +1287,14 @@
       <c r="B10" s="3">
         <v>37</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="17">
         <v>220</v>
       </c>
-      <c r="E10" s="16">
-        <v>45362</v>
+      <c r="E10" s="14">
+        <v>45361</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,14 +1304,14 @@
       <c r="B11" s="3">
         <v>24</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="17">
         <v>150</v>
       </c>
-      <c r="E11" s="16">
-        <v>45393</v>
+      <c r="E11" s="14">
+        <v>45392</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,14 +1321,14 @@
       <c r="B12" s="3">
         <v>29</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="17">
         <v>100</v>
       </c>
-      <c r="E12" s="16">
-        <v>45393</v>
+      <c r="E12" s="14">
+        <v>45392</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,14 +1338,14 @@
       <c r="B13" s="3">
         <v>32</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="17">
         <v>200</v>
       </c>
-      <c r="E13" s="16">
-        <v>45423</v>
+      <c r="E13" s="14">
+        <v>45392</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,14 +1355,14 @@
       <c r="B14" s="3">
         <v>27</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="17">
         <v>220</v>
       </c>
-      <c r="E14" s="16">
-        <v>45423</v>
+      <c r="E14" s="14">
+        <v>45422</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,14 +1372,14 @@
       <c r="B15" s="3">
         <v>35</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="17">
         <v>190</v>
       </c>
-      <c r="E15" s="16">
-        <v>45423</v>
+      <c r="E15" s="14">
+        <v>45422</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,14 +1389,14 @@
       <c r="B16" s="3">
         <v>20</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="17">
         <v>180</v>
       </c>
-      <c r="E16" s="16">
-        <v>45454</v>
+      <c r="E16" s="14">
+        <v>45422</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1035,14 +1406,14 @@
       <c r="B17" s="3">
         <v>33</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="17">
         <v>200</v>
       </c>
-      <c r="E17" s="16">
-        <v>45454</v>
+      <c r="E17" s="14">
+        <v>45453</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,14 +1423,14 @@
       <c r="B18" s="3">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="17">
         <v>100</v>
       </c>
-      <c r="E18" s="16">
-        <v>45454</v>
+      <c r="E18" s="14">
+        <v>45453</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,14 +1440,14 @@
       <c r="B19" s="3">
         <v>36</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="17">
         <v>220</v>
       </c>
-      <c r="E19" s="16">
-        <v>45484</v>
+      <c r="E19" s="14">
+        <v>45453</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1086,14 +1457,14 @@
       <c r="B20" s="3">
         <v>23</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="17">
         <v>150</v>
       </c>
-      <c r="E20" s="16">
-        <v>45484</v>
+      <c r="E20" s="14">
+        <v>45483</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1103,14 +1474,14 @@
       <c r="B21" s="3">
         <v>31</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="17">
         <v>200</v>
       </c>
-      <c r="E21" s="16">
-        <v>45484</v>
+      <c r="E21" s="14">
+        <v>45483</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,14 +1491,14 @@
       <c r="B22" s="3">
         <v>27</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="17">
         <v>150</v>
       </c>
-      <c r="E22" s="16">
-        <v>45484</v>
+      <c r="E22" s="14">
+        <v>45483</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,14 +1508,14 @@
       <c r="B23" s="3">
         <v>22</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="17">
         <v>200</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>71</v>
+      <c r="E23" s="14">
+        <v>45514</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,14 +1525,14 @@
       <c r="B24" s="3">
         <v>35</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="17">
         <v>220</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>71</v>
+      <c r="E24" s="14">
+        <v>45514</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1171,14 +1542,14 @@
       <c r="B25" s="3">
         <v>18</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="17">
         <v>180</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>71</v>
+      <c r="E25" s="14">
+        <v>45514</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,14 +1559,14 @@
       <c r="B26" s="3">
         <v>31</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="17">
         <v>190</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>72</v>
+      <c r="E26" s="14">
+        <v>45545</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1205,14 +1576,14 @@
       <c r="B27" s="3">
         <v>25</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="17">
         <v>100</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>72</v>
+      <c r="E27" s="14">
+        <v>45545</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,14 +1593,14 @@
       <c r="B28" s="3">
         <v>33</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="17">
         <v>220</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>72</v>
+      <c r="E28" s="14">
+        <v>45545</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,14 +1610,14 @@
       <c r="B29" s="3">
         <v>30</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="17">
         <v>150</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>73</v>
+      <c r="E29" s="14">
+        <v>45575</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1256,14 +1627,14 @@
       <c r="B30" s="3">
         <v>20</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="17">
         <v>200</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>73</v>
+      <c r="E30" s="14">
+        <v>45575</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,14 +1644,14 @@
       <c r="B31" s="3">
         <v>29</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="17">
         <v>100</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>73</v>
+      <c r="E31" s="14">
+        <v>45575</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,14 +1661,14 @@
       <c r="B32" s="3">
         <v>26</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="17">
         <v>180</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>74</v>
+      <c r="E32" s="14">
+        <v>45606</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,14 +1678,14 @@
       <c r="B33" s="3">
         <v>19</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="17">
         <v>190</v>
       </c>
-      <c r="E33" s="16" t="s">
-        <v>74</v>
+      <c r="E33" s="14">
+        <v>45606</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1324,14 +1695,14 @@
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="17">
         <v>220</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>74</v>
+      <c r="E34" s="14">
+        <v>45606</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,14 +1712,14 @@
       <c r="B35" s="3">
         <v>24</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="17">
         <v>200</v>
       </c>
-      <c r="E35" s="16" t="s">
-        <v>75</v>
+      <c r="E35" s="14">
+        <v>45636</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,14 +1729,14 @@
       <c r="B36" s="3">
         <v>36</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="17">
         <v>180</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>75</v>
+      <c r="E36" s="14">
+        <v>45636</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,14 +1746,14 @@
       <c r="B37" s="3">
         <v>28</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="17">
         <v>100</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>75</v>
+      <c r="E37" s="14">
+        <v>45636</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,14 +1763,14 @@
       <c r="B38" s="3">
         <v>40</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="17">
         <v>190</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>76</v>
+      <c r="E38" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,14 +1780,14 @@
       <c r="B39" s="3">
         <v>23</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="17">
         <v>150</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>76</v>
+      <c r="E39" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,14 +1797,14 @@
       <c r="B40" s="3">
         <v>32</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="17">
         <v>220</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>76</v>
+      <c r="E40" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,14 +1814,14 @@
       <c r="B41" s="3">
         <v>34</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="17">
         <v>200</v>
       </c>
-      <c r="E41" s="16" t="s">
-        <v>77</v>
+      <c r="E41" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1460,14 +1831,14 @@
       <c r="B42" s="3">
         <v>27</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="17">
         <v>100</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>77</v>
+      <c r="E42" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,14 +1848,14 @@
       <c r="B43" s="3">
         <v>25</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="17">
         <v>150</v>
       </c>
-      <c r="E43" s="16" t="s">
-        <v>77</v>
+      <c r="E43" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1494,14 +1865,14 @@
       <c r="B44" s="3">
         <v>38</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="17">
         <v>220</v>
       </c>
-      <c r="E44" s="16" t="s">
-        <v>78</v>
+      <c r="E44" s="14" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1511,14 +1882,14 @@
       <c r="B45" s="3">
         <v>21</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="17">
         <v>190</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>78</v>
+      <c r="E45" s="14" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,14 +1899,14 @@
       <c r="B46" s="3">
         <v>35</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="17">
         <v>200</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>78</v>
+      <c r="E46" s="14" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,14 +1916,14 @@
       <c r="B47" s="3">
         <v>29</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="17">
         <v>180</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>79</v>
+      <c r="E47" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1562,14 +1933,14 @@
       <c r="B48" s="3">
         <v>26</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="17">
         <v>100</v>
       </c>
-      <c r="E48" s="16" t="s">
-        <v>79</v>
+      <c r="E48" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1579,14 +1950,14 @@
       <c r="B49" s="3">
         <v>24</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="17">
         <v>150</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>79</v>
+      <c r="E49" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,14 +1967,14 @@
       <c r="B50" s="3">
         <v>30</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="17">
         <v>190</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>80</v>
+      <c r="E50" s="14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,14 +1984,745 @@
       <c r="B51" s="3">
         <v>33</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="17">
         <v>220</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="3">
+        <v>31</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="17">
+        <v>220</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="3">
+        <v>40</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="17">
+        <v>220</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="3">
+        <v>29</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="17">
+        <v>220</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="3">
+        <v>34</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="17">
+        <v>200</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3">
+        <v>38</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="17">
+        <v>220</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="3">
+        <v>32</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57" s="17">
+        <v>200</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="3">
+        <v>26</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="17">
+        <v>180</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>80</v>
+      </c>
+      <c r="B59" s="3">
+        <v>30</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" s="17">
+        <v>200</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="3">
+        <v>40</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="17">
+        <v>220</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="3">
+        <v>31</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="17">
+        <v>150</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="3">
+        <v>33</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62" s="17">
+        <v>100</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="3">
+        <v>29</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" s="17">
+        <v>190</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="3">
+        <v>32</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" s="17">
+        <v>200</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="3">
+        <v>35</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="17">
+        <v>220</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="3">
+        <v>38</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="17">
+        <v>100</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="3">
+        <v>41</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="17">
+        <v>200</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="3">
+        <v>30</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="17">
+        <v>220</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="3">
+        <v>28</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" s="17">
+        <v>150</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70" s="3">
+        <v>37</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" s="17">
+        <v>190</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="3">
+        <v>31</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71" s="17">
+        <v>100</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="3">
+        <v>30</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="17">
+        <v>180</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="3">
+        <v>32</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" s="17">
+        <v>200</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="3">
+        <v>34</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D74" s="17">
+        <v>220</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="3">
+        <v>30</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="17">
+        <v>100</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="3">
+        <v>33</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="17">
+        <v>200</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="3">
+        <v>30</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" s="17">
+        <v>220</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78" s="3">
+        <v>28</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" s="17">
+        <v>180</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" s="3">
+        <v>31</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="17">
+        <v>190</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="3">
+        <v>40</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80" s="17">
+        <v>200</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="3">
+        <v>30</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="17">
+        <v>220</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="3">
+        <v>32</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="17">
+        <v>180</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="3">
+        <v>33</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" s="17">
+        <v>100</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="3">
+        <v>29</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D84" s="17">
+        <v>200</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="3">
+        <v>40</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" s="17">
+        <v>220</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" s="3">
+        <v>31</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86" s="17">
+        <v>200</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="3">
+        <v>32</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D87" s="17">
+        <v>190</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" s="3">
+        <v>34</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D88" s="17">
+        <v>100</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" s="3">
+        <v>30</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D89" s="17">
+        <v>220</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="3">
+        <v>35</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90" s="17">
+        <v>150</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" s="3">
+        <v>33</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D91" s="17">
+        <v>180</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" s="3">
+        <v>40</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92" s="17">
+        <v>200</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93" s="3">
+        <v>30</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D93" s="17">
+        <v>220</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="3">
+        <v>31</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D94" s="17">
+        <v>100</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1629,4 +2731,1039 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2F4C4C-6953-4C2D-95DC-DE10A35B351A}">
+  <dimension ref="A1:F59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="3">
+        <v>36</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="20">
+        <v>200</v>
+      </c>
+      <c r="E2" s="21">
+        <v>45302</v>
+      </c>
+      <c r="F2" s="23">
+        <f>SUM(D2:D59)</f>
+        <v>10110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3">
+        <v>33</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="20">
+        <v>190</v>
+      </c>
+      <c r="E3" s="21">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="3">
+        <v>29</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="20">
+        <v>180</v>
+      </c>
+      <c r="E4" s="21">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="3">
+        <v>30</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="20">
+        <v>220</v>
+      </c>
+      <c r="E5" s="21">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="3">
+        <v>40</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="20">
+        <v>100</v>
+      </c>
+      <c r="E6" s="21">
+        <v>45333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="20">
+        <v>200</v>
+      </c>
+      <c r="E7" s="21">
+        <v>45333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="3">
+        <v>32</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="20">
+        <v>180</v>
+      </c>
+      <c r="E8" s="21">
+        <v>45333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="3">
+        <v>33</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="20">
+        <v>200</v>
+      </c>
+      <c r="E9" s="21">
+        <v>45333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="3">
+        <v>28</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="20">
+        <v>150</v>
+      </c>
+      <c r="E10" s="21">
+        <v>45333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="3">
+        <v>30</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="20">
+        <v>100</v>
+      </c>
+      <c r="E11" s="21">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="3">
+        <v>32</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="20">
+        <v>200</v>
+      </c>
+      <c r="E12" s="21">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="3">
+        <v>36</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="20">
+        <v>200</v>
+      </c>
+      <c r="E13" s="21">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="3">
+        <v>31</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="20">
+        <v>200</v>
+      </c>
+      <c r="E14" s="21">
+        <v>45423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="3">
+        <v>34</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="20">
+        <v>220</v>
+      </c>
+      <c r="E15" s="21">
+        <v>45423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="3">
+        <v>33</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="20">
+        <v>100</v>
+      </c>
+      <c r="E16" s="21">
+        <v>45423</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="3">
+        <v>30</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="20">
+        <v>200</v>
+      </c>
+      <c r="E17" s="21">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="3">
+        <v>37</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="20">
+        <v>200</v>
+      </c>
+      <c r="E18" s="21">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="3">
+        <v>31</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="20">
+        <v>200</v>
+      </c>
+      <c r="E19" s="21">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3">
+        <v>28</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="17">
+        <v>150</v>
+      </c>
+      <c r="E20" s="21">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3">
+        <v>30</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="17">
+        <v>100</v>
+      </c>
+      <c r="E21" s="21">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3">
+        <v>31</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="17">
+        <v>220</v>
+      </c>
+      <c r="E22" s="21">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3">
+        <v>23</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="17">
+        <v>150</v>
+      </c>
+      <c r="E23" s="21">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3">
+        <v>31</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="17">
+        <v>200</v>
+      </c>
+      <c r="E24" s="21">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3">
+        <v>25</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="17">
+        <v>150</v>
+      </c>
+      <c r="E25" s="21">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="3">
+        <v>38</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="17">
+        <v>220</v>
+      </c>
+      <c r="E26" s="21">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3">
+        <v>21</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="17">
+        <v>190</v>
+      </c>
+      <c r="E27" s="21">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3">
+        <v>35</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="17">
+        <v>200</v>
+      </c>
+      <c r="E28" s="21">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="3">
+        <v>29</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="17">
+        <v>180</v>
+      </c>
+      <c r="E29" s="21">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3">
+        <v>26</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="17">
+        <v>100</v>
+      </c>
+      <c r="E30" s="21">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="3">
+        <v>41</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="17">
+        <v>200</v>
+      </c>
+      <c r="E31" s="21">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="3">
+        <v>32</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="17">
+        <v>180</v>
+      </c>
+      <c r="E32" s="21">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="3">
+        <v>30</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="17">
+        <v>200</v>
+      </c>
+      <c r="E33" s="21">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="3">
+        <v>30</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="17">
+        <v>200</v>
+      </c>
+      <c r="E34" s="21">
+        <v>45607</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="3">
+        <v>30</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="17">
+        <v>200</v>
+      </c>
+      <c r="E35" s="21">
+        <v>45607</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3">
+        <v>34</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="17">
+        <v>100</v>
+      </c>
+      <c r="E36" s="21">
+        <v>45637</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3">
+        <v>30</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="17">
+        <v>180</v>
+      </c>
+      <c r="E37" s="21">
+        <v>45637</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="3">
+        <v>21</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="17">
+        <v>220</v>
+      </c>
+      <c r="E38" s="21">
+        <v>45637</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="3">
+        <v>40</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="17">
+        <v>200</v>
+      </c>
+      <c r="E39" s="21">
+        <v>45637</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3">
+        <v>25</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="17">
+        <v>190</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3">
+        <v>30</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="17">
+        <v>180</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3">
+        <v>30</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="17">
+        <v>220</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3">
+        <v>30</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="17">
+        <v>150</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3">
+        <v>30</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="17">
+        <v>100</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="25">
+        <v>30</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="26">
+        <v>150</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="25">
+        <v>32</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="26">
+        <v>140</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" s="25">
+        <v>30</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="26">
+        <v>190</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="25">
+        <v>28</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="26">
+        <v>180</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="25">
+        <v>30</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="26">
+        <v>100</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="25">
+        <v>31</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="26">
+        <v>220</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="25">
+        <v>30</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="26">
+        <v>190</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="25">
+        <v>29</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="26">
+        <v>160</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="25">
+        <v>30</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="26">
+        <v>100</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="25">
+        <v>30</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="26">
+        <v>150</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="25">
+        <v>30</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="26">
+        <v>190</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="25">
+        <v>30</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="26">
+        <v>200</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" s="25">
+        <v>33</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="26">
+        <v>150</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B58" s="25">
+        <v>30</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="26">
+        <v>190</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" s="25">
+        <v>30</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="26">
+        <v>180</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E43" xr:uid="{AF2F4C4C-6953-4C2D-95DC-DE10A35B351A}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>